<commit_message>
Add system tests for follows
</commit_message>
<xml_diff>
--- a/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test1/QuerySet1.xlsx
+++ b/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test1/QuerySet1.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="154">
   <si>
     <t>Index</t>
   </si>
@@ -85,99 +85,51 @@
     <t>All varables</t>
   </si>
   <si>
-    <t>Select SingleSynonym Follows IntInt HaveResult</t>
-  </si>
-  <si>
     <t>Select s such that Follows(1, _)</t>
   </si>
   <si>
-    <t>Select SingleSynonym Follows IntUnderscore HaveResult</t>
-  </si>
-  <si>
     <t>Select s such that Follows(1, s)</t>
   </si>
   <si>
-    <t>Select SingleSynonym Follows IntSynonym HaveResult</t>
-  </si>
-  <si>
-    <t>Select SingleSynonym Follows IntInt NoResult</t>
-  </si>
-  <si>
     <t>Select s such that Follows(3, s)</t>
   </si>
   <si>
-    <t>Select SingleSynonym Follows IntSynonym BehindWhile HaveResult</t>
-  </si>
-  <si>
     <t>Select s such that Follows(_, 3)</t>
   </si>
   <si>
-    <t>Select SingleSynonym Follows UnderscoreInt HaveResult</t>
-  </si>
-  <si>
     <t>Select s such that Follows(_, 1)</t>
   </si>
   <si>
-    <t>Select SingleSynonym Follows UnderscoreInt NoResult</t>
-  </si>
-  <si>
     <t>Select s such that Follows(_, _)</t>
   </si>
   <si>
-    <t>Select SingleSynonym Follows UnderscoreUnderscore HaveResult</t>
-  </si>
-  <si>
     <t>Select s such that Follows(_, s)</t>
   </si>
   <si>
-    <t>Select SingleSynonym Follows UnderscoreSynonym HaveResult</t>
-  </si>
-  <si>
     <t>Select s such that Follows(s, 2)</t>
   </si>
   <si>
-    <t>Select SingleSynonym Follows SynonymInt HaveResult</t>
-  </si>
-  <si>
-    <t>Select SingleSynonym Follows SynonymInt NoResult</t>
-  </si>
-  <si>
     <t>Select s such that Follows(s, 1)</t>
   </si>
   <si>
     <t>Select s such that Follows(s, 8)</t>
   </si>
   <si>
-    <t>Select SingleSynonym Follows SynonymInt BeforeWhile HaveResult</t>
-  </si>
-  <si>
     <t>Select s such that Follows(s, _)</t>
   </si>
   <si>
-    <t>Select SingleSynonym Follows SynonymUnderscore HaveResult</t>
-  </si>
-  <si>
     <t>stmt s1, s2;</t>
   </si>
   <si>
     <t>Select s1 such that Follows(s1, s2)</t>
   </si>
   <si>
-    <t>Select SingleSynonym Follows SynonymSynonym GetFront HaveResult</t>
-  </si>
-  <si>
-    <t>Select SingleSynonym Follows SynonymSynonym GetBack HaveResult</t>
-  </si>
-  <si>
     <t>Select s2 such that Follows(s1, s2)</t>
   </si>
   <si>
     <t>Select s such that Follows(s, s)</t>
   </si>
   <si>
-    <t>Select SingleSynonym Follows SynonymUnderscore NoResult</t>
-  </si>
-  <si>
     <t>stmts;</t>
   </si>
   <si>
@@ -194,13 +146,352 @@
   </si>
   <si>
     <t>1,2,3,4,5,6</t>
+  </si>
+  <si>
+    <t>Select v such that Follows(1, 2)</t>
+  </si>
+  <si>
+    <t>Select v such that Follows(3, 4)</t>
+  </si>
+  <si>
+    <t>Select v such that Follows(1, _)</t>
+  </si>
+  <si>
+    <t>Select v such that Follows(1, s)</t>
+  </si>
+  <si>
+    <t>Select v such that Follows(3, s)</t>
+  </si>
+  <si>
+    <t>Select v such that Follows(_, 3)</t>
+  </si>
+  <si>
+    <t>Select v such that Follows(_, 1)</t>
+  </si>
+  <si>
+    <t>Select v such that Follows(_, _)</t>
+  </si>
+  <si>
+    <t>Select v such that Follows(_, s)</t>
+  </si>
+  <si>
+    <t>Select v such that Follows(s, 2)</t>
+  </si>
+  <si>
+    <t>Select v such that Follows(s, 1)</t>
+  </si>
+  <si>
+    <t>Select v such that Follows(s, 8)</t>
+  </si>
+  <si>
+    <t>Select v such that Follows(s, _)</t>
+  </si>
+  <si>
+    <t>Select v such that Follows(v, s)</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Variable Follows IntInt HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Variable Follows IntInt NoResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Variable Follows IntUnderscore HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Variable Follows IntSynonym HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Variable Follows IntSynonym BehindWhile HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Variable Follows UnderscoreInt HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Variable Follows UnderscoreInt NoResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Variable Follows UnderscoreUnderscore HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Variable Follows UnderscoreSynonym HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Variable Follows SynonymInt HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Variable Follows SynonymInt NoResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Variable Follows SynonymInt BeforeWhile HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Variable Follows SynonymUnderscore HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Variable Follows Illegal Argument NoResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows IntInt HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows IntInt NoResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows IntUnderscore HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows IntSynonym HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows IntSynonym BehindWhile HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows UnderscoreInt HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows UnderscoreInt NoResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows UnderscoreUnderscore HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows UnderscoreSynonym HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows SynonymInt HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows SynonymInt NoResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows SynonymInt BeforeWhile HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows SynonymUnderscore HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows SynonymSynonym GetFront HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows SynonymSynonym GetBack HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows SynonymUnderscore NoResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Assign Follows IntInt HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Assign Follows IntInt NoResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Assign Follows IntUnderscore HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Assign Follows IntSynonym HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Assign Follows IntSynonym BehindWhile HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Assign Follows UnderscoreInt HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Assign Follows UnderscoreInt NoResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Assign Follows UnderscoreUnderscore HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Assign Follows UnderscoreSynonym HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Assign Follows SynonymInt HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Assign Follows SynonymInt NoResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Assign Follows SynonymUnderscore HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Assign Follows SynonymSynonym GetFront HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Assign Follows SynonymSynonym GetBack HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Assign Follows SynonymUnderscore NoResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym While Follows IntInt HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym While Follows IntInt NoResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym While Follows IntUnderscore HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym While Follows IntSynonym HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym While Follows UnderscoreInt HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym While Follows UnderscoreInt NoResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym While Follows UnderscoreUnderscore HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym While Follows UnderscoreSynonym HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym While Follows SynonymInt HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym While Follows SynonymInt NoResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym While Follows SynonymUnderscore HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym While Follows SynonymUnderscore NoResult</t>
+  </si>
+  <si>
+    <t>assign a1, a2;</t>
+  </si>
+  <si>
+    <t>while w1, w2;</t>
+  </si>
+  <si>
+    <t>Select w such that Follows(1, 2)</t>
+  </si>
+  <si>
+    <t>Select w such that Follows(3, 4)</t>
+  </si>
+  <si>
+    <t>Select w such that Follows(1, _)</t>
+  </si>
+  <si>
+    <t>Select w such that Follows(3, w)</t>
+  </si>
+  <si>
+    <t>Select w such that Follows(_, 3)</t>
+  </si>
+  <si>
+    <t>Select w such that Follows(_, 1)</t>
+  </si>
+  <si>
+    <t>Select w such that Follows(_, _)</t>
+  </si>
+  <si>
+    <t>Select w such that Follows(_, w)</t>
+  </si>
+  <si>
+    <t>Select w such that Follows(w, 1)</t>
+  </si>
+  <si>
+    <t>Select w such that Follows(w, 8)</t>
+  </si>
+  <si>
+    <t>Select w such that Follows(w, _)</t>
+  </si>
+  <si>
+    <t>Select w1 such that Follows(w1, w2)</t>
+  </si>
+  <si>
+    <t>Select w2 such that Follows(w1, w2)</t>
+  </si>
+  <si>
+    <t>Select w such that Follows(w, w)</t>
+  </si>
+  <si>
+    <t>Select a such that Follows(1, 2)</t>
+  </si>
+  <si>
+    <t>Select a such that Follows(3, 4)</t>
+  </si>
+  <si>
+    <t>Select a such that Follows(1, _)</t>
+  </si>
+  <si>
+    <t>Select a such that Follows(1, a)</t>
+  </si>
+  <si>
+    <t>Select a such that Follows(3, a)</t>
+  </si>
+  <si>
+    <t>Select a such that Follows(_, 3)</t>
+  </si>
+  <si>
+    <t>Select a such that Follows(_, 1)</t>
+  </si>
+  <si>
+    <t>Select a such that Follows(_, _)</t>
+  </si>
+  <si>
+    <t>Select a such that Follows(_, a)</t>
+  </si>
+  <si>
+    <t>Select a such that Follows(a, 2)</t>
+  </si>
+  <si>
+    <t>Select a such that Follows(a, 1)</t>
+  </si>
+  <si>
+    <t>Select a such that Follows(a, 8)</t>
+  </si>
+  <si>
+    <t>Select a such that Follows(a, _)</t>
+  </si>
+  <si>
+    <t>Select a1 such that Follows(a1, a2)</t>
+  </si>
+  <si>
+    <t>Select a2 such that Follows(a1, a2)</t>
+  </si>
+  <si>
+    <t>Select a such that Follows(a, a)</t>
+  </si>
+  <si>
+    <t>variable v; stmt s;</t>
+  </si>
+  <si>
+    <t>2,5,6,7,8</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Assign Follows SynonymInt BeforeIntNotAssign NoResult</t>
+  </si>
+  <si>
+    <t>1,2,4,5,6</t>
+  </si>
+  <si>
+    <t>1,4,5,6</t>
+  </si>
+  <si>
+    <t>2,5,6,7</t>
+  </si>
+  <si>
+    <t>Select w such that Follows(2, w)</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym While Follows IntSynonym WhileFollowItself NoResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym While Follows SynonymSynonym GetFront NoResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym While Follows SynonymSynonym GetBack NoResult</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,6 +514,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -257,7 +556,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -271,18 +570,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -601,16 +904,16 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="7" t="s">
         <v>16</v>
       </c>
     </row>
@@ -641,7 +944,7 @@
       <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="8">
         <v>3</v>
       </c>
       <c r="E4" t="s">
@@ -672,309 +975,1074 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.85546875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="52.140625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="6" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.85546875" style="10" customWidth="1"/>
+    <col min="3" max="3" width="52.140625" style="10" customWidth="1"/>
     <col min="4" max="4" width="35.42578125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="66" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="6"/>
+    <col min="5" max="5" width="66" style="10" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="13" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>52</v>
+      <c r="C2" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
+      <c r="D4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C5" s="10" t="s">
         <v>21</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="D5" s="11">
         <v>2</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>24</v>
+      <c r="E5" s="10" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="9">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>26</v>
+      <c r="C6" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="D6" s="11">
         <v>8</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>27</v>
+      <c r="E6" s="10" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="9">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>28</v>
+      <c r="C7" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>29</v>
+      <c r="E7" s="10" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="9">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>31</v>
+      <c r="C8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="9">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>32</v>
+      <c r="C9" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>33</v>
+      <c r="E9" s="10" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="9">
         <v>9</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>35</v>
+      <c r="C10" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="9">
         <v>10</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>36</v>
+      <c r="C11" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D11" s="11">
         <v>1</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>37</v>
+      <c r="E11" s="10" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+      <c r="A12" s="9">
         <v>11</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="9" t="s">
+      <c r="C12" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>38</v>
       </c>
+      <c r="E12" s="10" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+      <c r="A13" s="9">
         <v>12</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>40</v>
+      <c r="C13" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="D13" s="11">
         <v>3</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>13</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>14</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>15</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>16</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>17</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>13</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="9" t="s">
+      <c r="D18" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <v>18</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D19" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="9" t="s">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
+        <v>19</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+      <c r="D20" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
+        <v>20</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
+        <v>21</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="9">
+        <v>22</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
+        <v>23</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="9">
+        <v>24</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
+        <v>25</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="9">
+        <v>26</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="9">
+        <v>27</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="9">
+        <v>28</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="9">
+        <v>29</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="9">
+        <v>30</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="9">
+        <v>31</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="D32" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="E32" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="9">
+        <v>32</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="9">
+        <v>33</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="9">
+        <v>34</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="D35" s="11">
+        <v>2</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="9">
+        <v>35</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="D36" s="11">
+        <v>8</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="9">
+        <v>36</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="9">
+        <v>37</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="9">
+        <v>38</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="9">
+        <v>39</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="9">
+        <v>40</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="D41" s="11">
+        <v>1</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="9">
+        <v>41</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="9">
+        <v>42</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="9">
+        <v>43</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="9">
         <v>44</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="B45" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="9">
         <v>45</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="B46" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="9">
+        <v>46</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="9">
+        <v>47</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D48" s="11">
+        <v>3</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="9">
+        <v>48</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="9">
+        <v>49</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D50" s="11">
+        <v>3</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="9">
+        <v>50</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="D51" s="11">
+        <v>3</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="9">
+        <v>51</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="9">
+        <v>52</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="D53" s="11">
+        <v>3</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="9">
+        <v>53</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="9">
+        <v>54</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D55" s="11">
+        <v>3</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="9">
+        <v>55</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D56" s="11">
+        <v>3</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="9">
         <v>56</v>
       </c>
-      <c r="E15" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
-        <v>15</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
-        <v>16</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>50</v>
+      <c r="B57" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D57" s="11">
+        <v>3</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="9">
+        <v>57</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="9">
+        <v>59</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D59" s="11">
+        <v>3</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="9">
+        <v>60</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="9">
+        <v>61</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D61" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="9">
+        <v>62</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="D62" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1082,28 +2150,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update AutoTester bat file
</commit_message>
<xml_diff>
--- a/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test1/QuerySet1.xlsx
+++ b/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test1/QuerySet1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Complex" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="156">
   <si>
     <t>Index</t>
   </si>
@@ -485,13 +485,19 @@
   </si>
   <si>
     <t>Select SingleSynonym While Follows SynonymSynonym GetBack NoResult</t>
+  </si>
+  <si>
+    <t>aaaa</t>
+  </si>
+  <si>
+    <t>hello test test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -535,6 +541,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -556,7 +569,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -570,10 +583,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -586,6 +595,13 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -868,104 +884,113 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3B02F3-8668-4835-B18A-9EFEA275CE21}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
-    <col min="3" max="3" width="37.140625" customWidth="1"/>
-    <col min="4" max="4" width="39.7109375" customWidth="1"/>
-    <col min="5" max="5" width="35.85546875" customWidth="1"/>
+    <col min="1" max="1" width="6" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" style="14" customWidth="1"/>
+    <col min="3" max="3" width="37.140625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="39.7109375" style="14" customWidth="1"/>
+    <col min="5" max="5" width="35.85546875" style="14" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="14" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="14" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="13">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="15">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="14" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5" s="13">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="14" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -977,1071 +1002,1071 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.85546875" style="10" customWidth="1"/>
-    <col min="3" max="3" width="52.140625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="35.42578125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="66" style="10" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="1" width="6" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.85546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="52.140625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="66" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="11" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="8" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="8" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="8" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="9">
         <v>2</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="8" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="9">
         <v>8</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="8" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+      <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="8" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+      <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="8" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+      <c r="A10" s="7">
         <v>9</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="8" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+      <c r="A11" s="7">
         <v>10</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="9">
         <v>1</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="8" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+      <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="8" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
+      <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="9">
         <v>3</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="8" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="A14" s="7">
         <v>13</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="8" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
+      <c r="A15" s="7">
         <v>14</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="8" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
+      <c r="A16" s="7">
         <v>15</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="8" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
+      <c r="A17" s="7">
         <v>16</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="8" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
+      <c r="A18" s="7">
         <v>17</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="8" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
+      <c r="A19" s="7">
         <v>18</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
+      <c r="A20" s="7">
         <v>19</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="8" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
+      <c r="A21" s="7">
         <v>20</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="8" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
+      <c r="A22" s="7">
         <v>21</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
+      <c r="A23" s="7">
         <v>22</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="8" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="9">
+      <c r="A24" s="7">
         <v>23</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="8" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="9">
+      <c r="A25" s="7">
         <v>24</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="8" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="9">
+      <c r="A26" s="7">
         <v>25</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="D26" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="8" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="9">
+      <c r="A27" s="7">
         <v>26</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D27" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="8" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="9">
+      <c r="A28" s="7">
         <v>27</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D28" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="8" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="9">
+      <c r="A29" s="7">
         <v>28</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E29" s="8" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="9">
+      <c r="A30" s="7">
         <v>29</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="D30" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="E30" s="8" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="9">
+      <c r="A31" s="7">
         <v>30</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D31" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E31" s="8" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="9">
+      <c r="A32" s="7">
         <v>31</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D32" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="8" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="9">
+      <c r="A33" s="7">
         <v>32</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="D33" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E33" s="8" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="9">
+      <c r="A34" s="7">
         <v>33</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="D34" s="11" t="s">
+      <c r="D34" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="E34" s="8" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="9">
+      <c r="A35" s="7">
         <v>34</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="D35" s="11">
+      <c r="D35" s="9">
         <v>2</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E35" s="8" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="9">
+      <c r="A36" s="7">
         <v>35</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C36" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="D36" s="11">
+      <c r="D36" s="9">
         <v>8</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="E36" s="8" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="9">
+      <c r="A37" s="7">
         <v>36</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B37" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="D37" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E37" s="8" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="9">
+      <c r="A38" s="7">
         <v>37</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C38" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D38" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E38" s="10" t="s">
+      <c r="E38" s="8" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="9">
+      <c r="A39" s="7">
         <v>38</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B39" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C39" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="D39" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="E39" s="8" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="9">
+      <c r="A40" s="7">
         <v>39</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="B40" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="C40" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="D40" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="E40" s="8" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="9">
+      <c r="A41" s="7">
         <v>40</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C41" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="D41" s="11">
+      <c r="D41" s="9">
         <v>1</v>
       </c>
-      <c r="E41" s="10" t="s">
+      <c r="E41" s="8" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="9">
+      <c r="A42" s="7">
         <v>41</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="C42" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="D42" s="11" t="s">
+      <c r="D42" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E42" s="10" t="s">
+      <c r="E42" s="8" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="9">
+      <c r="A43" s="7">
         <v>42</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C43" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="D43" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E43" s="10" t="s">
+      <c r="E43" s="8" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="9">
+      <c r="A44" s="7">
         <v>43</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="B44" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="C44" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="D44" s="11" t="s">
+      <c r="D44" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="E44" s="10" t="s">
+      <c r="E44" s="8" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="9">
+      <c r="A45" s="7">
         <v>44</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="D45" s="11" t="s">
+      <c r="D45" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="E45" s="10" t="s">
+      <c r="E45" s="8" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="9">
+      <c r="A46" s="7">
         <v>45</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C46" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="D46" s="11" t="s">
+      <c r="D46" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E46" s="10" t="s">
+      <c r="E46" s="8" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="9">
+      <c r="A47" s="7">
         <v>46</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B47" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C47" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="D47" s="11" t="s">
+      <c r="D47" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E47" s="10" t="s">
+      <c r="E47" s="8" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="9">
+      <c r="A48" s="7">
         <v>47</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="B48" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="C48" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="D48" s="11">
+      <c r="D48" s="9">
         <v>3</v>
       </c>
-      <c r="E48" s="10" t="s">
+      <c r="E48" s="8" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="9">
+      <c r="A49" s="7">
         <v>48</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="B49" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="C49" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="D49" s="11" t="s">
+      <c r="D49" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E49" s="10" t="s">
+      <c r="E49" s="8" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="9">
+      <c r="A50" s="7">
         <v>49</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="B50" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="C50" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="D50" s="11">
+      <c r="D50" s="9">
         <v>3</v>
       </c>
-      <c r="E50" s="10" t="s">
+      <c r="E50" s="8" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="9">
+      <c r="A51" s="7">
         <v>50</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="B51" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="C51" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="D51" s="11">
+      <c r="D51" s="9">
         <v>3</v>
       </c>
-      <c r="E51" s="10" t="s">
+      <c r="E51" s="8" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="9">
+      <c r="A52" s="7">
         <v>51</v>
       </c>
-      <c r="B52" s="10" t="s">
+      <c r="B52" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C52" s="10" t="s">
+      <c r="C52" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="D52" s="11" t="s">
+      <c r="D52" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E52" s="10" t="s">
+      <c r="E52" s="8" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="9">
+      <c r="A53" s="7">
         <v>52</v>
       </c>
-      <c r="B53" s="10" t="s">
+      <c r="B53" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="C53" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="D53" s="11">
+      <c r="D53" s="9">
         <v>3</v>
       </c>
-      <c r="E53" s="10" t="s">
+      <c r="E53" s="8" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="9">
+      <c r="A54" s="7">
         <v>53</v>
       </c>
-      <c r="B54" s="10" t="s">
+      <c r="B54" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C54" s="10" t="s">
+      <c r="C54" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="D54" s="11" t="s">
+      <c r="D54" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E54" s="10" t="s">
+      <c r="E54" s="8" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="9">
+      <c r="A55" s="7">
         <v>54</v>
       </c>
-      <c r="B55" s="10" t="s">
+      <c r="B55" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C55" s="10" t="s">
+      <c r="C55" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="D55" s="11">
+      <c r="D55" s="9">
         <v>3</v>
       </c>
-      <c r="E55" s="10" t="s">
+      <c r="E55" s="8" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="9">
+      <c r="A56" s="7">
         <v>55</v>
       </c>
-      <c r="B56" s="10" t="s">
+      <c r="B56" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C56" s="10" t="s">
+      <c r="C56" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="D56" s="11">
+      <c r="D56" s="9">
         <v>3</v>
       </c>
-      <c r="E56" s="10" t="s">
+      <c r="E56" s="8" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="9">
+      <c r="A57" s="7">
         <v>56</v>
       </c>
-      <c r="B57" s="10" t="s">
+      <c r="B57" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C57" s="10" t="s">
+      <c r="C57" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="D57" s="11">
+      <c r="D57" s="9">
         <v>3</v>
       </c>
-      <c r="E57" s="10" t="s">
+      <c r="E57" s="8" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="9">
+      <c r="A58" s="7">
         <v>57</v>
       </c>
-      <c r="B58" s="10" t="s">
+      <c r="B58" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C58" s="10" t="s">
+      <c r="C58" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="D58" s="11" t="s">
+      <c r="D58" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E58" s="10" t="s">
+      <c r="E58" s="8" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="9">
+      <c r="A59" s="7">
         <v>59</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="B59" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C59" s="10" t="s">
+      <c r="C59" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="D59" s="11">
+      <c r="D59" s="9">
         <v>3</v>
       </c>
-      <c r="E59" s="10" t="s">
+      <c r="E59" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="9">
+      <c r="A60" s="7">
         <v>60</v>
       </c>
-      <c r="B60" s="10" t="s">
+      <c r="B60" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="C60" s="10" t="s">
+      <c r="C60" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="D60" s="11" t="s">
+      <c r="D60" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E60" s="10" t="s">
+      <c r="E60" s="8" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="9">
+      <c r="A61" s="7">
         <v>61</v>
       </c>
-      <c r="B61" s="10" t="s">
+      <c r="B61" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="C61" s="10" t="s">
+      <c r="C61" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="D61" s="11" t="s">
+      <c r="D61" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E61" s="10" t="s">
+      <c r="E61" s="8" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="9">
+      <c r="A62" s="7">
         <v>62</v>
       </c>
-      <c r="B62" s="10" t="s">
+      <c r="B62" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C62" s="10" t="s">
+      <c r="C62" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="D62" s="11" t="s">
+      <c r="D62" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E62" s="10" t="s">
+      <c r="E62" s="8" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add more Follows test cases
</commit_message>
<xml_diff>
--- a/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test1/QuerySet1.xlsx
+++ b/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test1/QuerySet1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Complex" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="267">
   <si>
     <t>Index</t>
   </si>
@@ -604,9 +604,6 @@
     <t>Follows (1, 2)</t>
   </si>
   <si>
-    <t>Missing SelectKeyword</t>
-  </si>
-  <si>
     <t>stmt s</t>
   </si>
   <si>
@@ -637,9 +634,6 @@
     <t>Select s Follows(1, 2)</t>
   </si>
   <si>
-    <t>Missing SuchThat Keyword</t>
-  </si>
-  <si>
     <t>stmt Follows;</t>
   </si>
   <si>
@@ -680,6 +674,156 @@
   </si>
   <si>
     <t>SuchThatKeyword StuckToFrontOf PreviousRelation NoResult</t>
+  </si>
+  <si>
+    <t>Missing SuchThat Keyword NoResult</t>
+  </si>
+  <si>
+    <t>Missing SelectKeyword NoResult</t>
+  </si>
+  <si>
+    <t>Select s such that Follows(1, _) and Follows(2, _)</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows IntUnderscore And Follows IntUnderscore HaveResult</t>
+  </si>
+  <si>
+    <t>Select s such that Follows(1, s) and Follows(2, s)</t>
+  </si>
+  <si>
+    <t>stmt s1, s2, s3;</t>
+  </si>
+  <si>
+    <t>Select s1 such that Follows(1, s2) and Follows(2, s3)</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows IntSynonym And Follows IntSynonym BothRelationSameSynonym NoResult</t>
+  </si>
+  <si>
+    <t>Select s1 such that Follows(1, s1) and Follows(2, s2)</t>
+  </si>
+  <si>
+    <t>Select s2 such that Follows(1, s1) and Follows(2, s2)</t>
+  </si>
+  <si>
+    <t>Select s such that Follows(_, 2) and Follows(_, 4)</t>
+  </si>
+  <si>
+    <t>Select s such that Follows(_, 2) and Follows(_, 5)</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows UnderscoreInt And Follows UnderscoreInt NoResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows UnderscoreInt And Follows UnderscoreInt HaveResult</t>
+  </si>
+  <si>
+    <t>Select s such that Follows(_, _) and Follows(_, _)</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows UnderscoreUnderscore And Follows UnderscoreUnderscore HaveResult</t>
+  </si>
+  <si>
+    <t>Select s such that Follows(_, s) and Follows(_, s)</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows UnderscoreSynonym And Follows UnderscoreSynonym CommonSynonym HaveResult</t>
+  </si>
+  <si>
+    <t>Select s1 such that Follows(_, s2) and Follows(_, s3)</t>
+  </si>
+  <si>
+    <t>Select s1 such that Follows(_, s1) and Follows(_, s2)</t>
+  </si>
+  <si>
+    <t>Select s2 such that Follows(_, s1) and Follows(_, s2)</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows UnderscoreSynonym And Follows UnderscoreSynonym UniqueSynonym HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows UnderscoreSynonym And Follows UnderscoreSynonym GetFront HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows UnderscoreSynonym And Follows UnderscoreSynonym GetBack HaveResult</t>
+  </si>
+  <si>
+    <t>Select s such that Follows(s, 2) and Follows(s, 3)</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows IntSynonym And Follows IntSynonym BothRelationDiffSynonym HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows IntSynonym And Follows IntSynonym GetFront HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows IntSynonym And Follows IntSynonym GetBack HaveResult</t>
+  </si>
+  <si>
+    <t>Select s1 such that Follows(s1, 2) and Follows(s2, 3)</t>
+  </si>
+  <si>
+    <t>Select s2 such that Follows(s1, 2) and Follows(s2, 3)</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows SynonymInt And Follows SynonymInt BothRelation SameSynonym NoResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows SynonymInt And Follows SynonymInt GetFront HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows SynonymInt And Follows SynonymInt GetBack HaveResult</t>
+  </si>
+  <si>
+    <t>Select s1 such that Follows(s1, _) and Follows(s2, _)</t>
+  </si>
+  <si>
+    <t>Select s2 such that Follows(s1, _) and Follows(s2, _)</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows SynonymUnderscore And Follows SynonymUnderscore GetFront HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows SynonymUnderscore And Follows SynonymUnderscore GetBack HaveResult</t>
+  </si>
+  <si>
+    <t>Select s1 such that Follows(s1, s2) and Follows(s2, s3)</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows SynonymSynonym And Follows SynonymSynonym Chain GetFirst HaveResult</t>
+  </si>
+  <si>
+    <t>Select s2 such that Follows(s1, s2) and Follows(s2, s3)</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows SynonymSynonym And Follows SynonymSynonym Chain GetMiddle HaveResult</t>
+  </si>
+  <si>
+    <t>Select s3 such that Follows(s1, s2) and Follows(s2, s3)</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows SynonymSynonym And Follows SynonymSynonym Chain GetLast HaveResult</t>
+  </si>
+  <si>
+    <t>Select s1 such that Follows(s1, s3) and Follows(s2, s3)</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows SynonymSynonym And Follows SynonymSynonym Chain s3ShldNotFollowTwice NoResult</t>
+  </si>
+  <si>
+    <t>Select s1 such that Follows(s1, s2) and Follows(s1, s3)</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Follows SynonymSynonym And Follows SynonymSynonym Chain s1ShldNotHaveTwoFollowers NoResult</t>
+  </si>
+  <si>
+    <t>1,2,4,5</t>
+  </si>
+  <si>
+    <t>2,3,5,6</t>
+  </si>
+  <si>
+    <t>3,6,7,8</t>
   </si>
 </sst>
 </file>
@@ -1103,8 +1247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3B02F3-8668-4835-B18A-9EFEA275CE21}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,7 +1351,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>12</v>
@@ -1216,7 +1360,7 @@
         <v>38</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1233,7 +1377,7 @@
         <v>38</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1275,16 +1419,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="C10" s="18" t="s">
         <v>199</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>200</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1295,13 +1439,13 @@
         <v>5</v>
       </c>
       <c r="C11" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="18" t="s">
         <v>197</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1309,10 +1453,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>38</v>
@@ -1382,6 +1526,9 @@
       <c r="C16" s="18" t="s">
         <v>154</v>
       </c>
+      <c r="D16" s="21" t="s">
+        <v>13</v>
+      </c>
       <c r="E16" s="18" t="s">
         <v>157</v>
       </c>
@@ -1396,6 +1543,9 @@
       <c r="C17" s="18" t="s">
         <v>155</v>
       </c>
+      <c r="D17" s="21" t="s">
+        <v>13</v>
+      </c>
       <c r="E17" s="18" t="s">
         <v>156</v>
       </c>
@@ -1408,10 +1558,13 @@
         <v>5</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>211</v>
+        <v>209</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>13</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -1422,10 +1575,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A80"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1434,7 +1587,7 @@
     <col min="2" max="2" width="54.85546875" style="8" customWidth="1"/>
     <col min="3" max="3" width="52.140625" style="8" customWidth="1"/>
     <col min="4" max="4" width="35.42578125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="66" style="8" customWidth="1"/>
+    <col min="5" max="5" width="127.7109375" style="8" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
@@ -1584,8 +1737,8 @@
       <c r="C9" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="D9" s="13" t="s">
-        <v>38</v>
+      <c r="D9" s="21" t="s">
+        <v>13</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>176</v>
@@ -1630,13 +1783,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="21" t="s">
         <v>205</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>206</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -1647,13 +1803,13 @@
         <v>5</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D13" s="21" t="s">
         <v>38</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -1669,8 +1825,8 @@
       <c r="D14" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="13" t="s">
-        <v>193</v>
+      <c r="E14" s="21" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1768,7 +1924,7 @@
       <c r="C20" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="22" t="s">
         <v>13</v>
       </c>
       <c r="E20" s="8" t="s">
@@ -1797,13 +1953,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="21" t="s">
         <v>208</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2700,6 +2859,9 @@
       <c r="C75" s="14" t="s">
         <v>158</v>
       </c>
+      <c r="D75" s="22" t="s">
+        <v>13</v>
+      </c>
       <c r="E75" s="14" t="s">
         <v>159</v>
       </c>
@@ -2714,6 +2876,9 @@
       <c r="C76" s="14" t="s">
         <v>177</v>
       </c>
+      <c r="D76" s="22" t="s">
+        <v>13</v>
+      </c>
       <c r="E76" s="14" t="s">
         <v>178</v>
       </c>
@@ -2726,13 +2891,13 @@
         <v>5</v>
       </c>
       <c r="C77" s="21" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D77" s="22" t="s">
         <v>38</v>
       </c>
       <c r="E77" s="21" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -2745,6 +2910,9 @@
       <c r="C78" s="14" t="s">
         <v>160</v>
       </c>
+      <c r="D78" s="22" t="s">
+        <v>13</v>
+      </c>
       <c r="E78" s="14" t="s">
         <v>161</v>
       </c>
@@ -2757,10 +2925,13 @@
         <v>5</v>
       </c>
       <c r="C79" s="21" t="s">
-        <v>213</v>
+        <v>211</v>
+      </c>
+      <c r="D79" s="22" t="s">
+        <v>13</v>
       </c>
       <c r="E79" s="21" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -2771,13 +2942,387 @@
         <v>5</v>
       </c>
       <c r="C80" s="21" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D80" s="22" t="s">
         <v>38</v>
       </c>
       <c r="E80" s="21" t="s">
-        <v>218</v>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="7">
+        <v>80</v>
+      </c>
+      <c r="B81" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="D81" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E81" s="21" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="7">
+        <v>81</v>
+      </c>
+      <c r="B82" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C82" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="D82" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E82" s="21" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="7">
+        <v>82</v>
+      </c>
+      <c r="B83" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="C83" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="D83" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E83" s="21" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="7">
+        <v>83</v>
+      </c>
+      <c r="B84" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C84" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="D84" s="9">
+        <v>2</v>
+      </c>
+      <c r="E84" s="21" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="7">
+        <v>84</v>
+      </c>
+      <c r="B85" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C85" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="D85" s="9">
+        <v>3</v>
+      </c>
+      <c r="E85" s="21" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="7">
+        <v>85</v>
+      </c>
+      <c r="B86" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C86" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="D86" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E86" s="21" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="7">
+        <v>86</v>
+      </c>
+      <c r="B87" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" s="21" t="s">
+        <v>227</v>
+      </c>
+      <c r="D87" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E87" s="21" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="7">
+        <v>87</v>
+      </c>
+      <c r="B88" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="D88" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E88" s="21" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="7">
+        <v>88</v>
+      </c>
+      <c r="B89" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C89" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="D89" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E89" s="21" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="7">
+        <v>89</v>
+      </c>
+      <c r="B90" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="C90" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="D90" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E90" s="21" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="7">
+        <v>90</v>
+      </c>
+      <c r="B91" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C91" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="D91" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E91" s="21" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="7">
+        <v>91</v>
+      </c>
+      <c r="B92" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C92" s="21" t="s">
+        <v>237</v>
+      </c>
+      <c r="D92" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E92" s="21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="7">
+        <v>92</v>
+      </c>
+      <c r="B93" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C93" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="D93" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E93" s="21" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="7">
+        <v>93</v>
+      </c>
+      <c r="B94" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C94" s="21" t="s">
+        <v>245</v>
+      </c>
+      <c r="D94" s="9">
+        <v>1</v>
+      </c>
+      <c r="E94" s="21" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="7">
+        <v>94</v>
+      </c>
+      <c r="B95" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C95" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="D95" s="9">
+        <v>2</v>
+      </c>
+      <c r="E95" s="21" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="7">
+        <v>95</v>
+      </c>
+      <c r="B96" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C96" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="D96" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E96" s="21" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="7">
+        <v>96</v>
+      </c>
+      <c r="B97" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C97" s="21" t="s">
+        <v>251</v>
+      </c>
+      <c r="D97" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E97" s="21" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="7">
+        <v>97</v>
+      </c>
+      <c r="B98" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="C98" s="21" t="s">
+        <v>254</v>
+      </c>
+      <c r="D98" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="E98" s="21" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="7">
+        <v>98</v>
+      </c>
+      <c r="B99" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="C99" s="21" t="s">
+        <v>256</v>
+      </c>
+      <c r="D99" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="E99" s="21" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="7">
+        <v>99</v>
+      </c>
+      <c r="B100" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="C100" s="21" t="s">
+        <v>258</v>
+      </c>
+      <c r="D100" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="E100" s="21" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="7">
+        <v>100</v>
+      </c>
+      <c r="B101" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="C101" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="D101" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E101" s="21" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="7">
+        <v>101</v>
+      </c>
+      <c r="B102" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="C102" s="21" t="s">
+        <v>262</v>
+      </c>
+      <c r="D102" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E102" s="21" t="s">
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>